<commit_message>
Added all papers citing the ARI as of February 5, 2021
</commit_message>
<xml_diff>
--- a/All ARI Papers/Affective_Reactivity_Index_Papers.xlsx
+++ b/All ARI Papers/Affective_Reactivity_Index_Papers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\string-mbd\RA Instruction Manuals\Lily Eisner\Research\ARI\ARI-Papers\All ARI Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9B2EBF-E8F4-47A2-94B5-D907F0506200}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBB93A3-D844-4559-BCA8-4FE26F0FFF1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5510" yWindow="80" windowWidth="12890" windowHeight="10070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3690" yWindow="730" windowWidth="14490" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="900">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="926">
   <si>
     <t>Authors</t>
   </si>
@@ -3468,6 +3468,100 @@
   </si>
   <si>
     <t>https://doi.org/10.1136/eb-2013-101400</t>
+  </si>
+  <si>
+    <t>Psychiatric comorbidity and social adjustment difficulties in children with disruptive mood dysregulation disorder: A national epidemiological study</t>
+  </si>
+  <si>
+    <t>Yu-Ju Lin, Wan-Ling Tseng, Susan Shur-Fen Gau</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jad.2020.12.039</t>
+  </si>
+  <si>
+    <t>Background
+We examined correlates, psychiatric comorbidities, and social adjustment difficulties in children with disruptive mood dysregulation disorder (DMDD) from a national epidemiological study in Taiwan.
+Methods
+The sample consisted of 4816 children, who were 3rd, 5th, and 7th graders from schools randomly chosen based on the urbanization level in a recent national survey of childhood mental disorders. Among the 4816 children (2520 boys, 52.3%) interviewed using the Kiddie epidemiologic version of the Schedule for Affective Disorders and Schizophrenia (K-SADS-E) for the DSM-5, 30 children were diagnosed as DMDD (23 boys, 76.7%). They and their parents also reported on the Social Adjustment Inventory for Children and Adolescents (SAICA). We conducted regressions for survey data that controlled for stratification and clustering.
+Results
+The weighted prevalence of DMDD was 0.3~0.76% in Taiwanese children. Lower parental educational levels, male predominance, higher psychiatric comorbidities, and worse self-report school functions (e.g., more behavioral problems with peers) were observed in children with DMDD than those without. Additional analyses revealed that oppositional defiant disorder (ODD) but not DMDD was related to conduct disorder. Children with ODD with or without DMDD had more problems regarding attitudes toward school, academic performance, and parent-child interaction at home than those with DMDD-only.
+Limitations
+Small sample size of DMDD.
+Conclusions
+DMDD is a rare disorder in the community. Children with DMDD had more psychiatric comorbidities, and subjectively experienced more difficulties than those without. DMDD and ODD both resulted in severe impairment yet in different domains.</t>
+  </si>
+  <si>
+    <t>Validation of an irritability measure in preschoolers in school-based and clinical Brazilian samples</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s00787-020-01701-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luisa Shiguemi Sugaya, Katharina Kircanski, Argyris Stringaris, Guilherme V. Polanczyk &amp; Ellen Leibenluft </t>
+  </si>
+  <si>
+    <t>The Affective Reactivity Index (ARI) is an irritability measure with good psychometric properties. However, there are no published studies in preschool children, an important population in which to differentiate normative from non-normative irritability. The goal of this study was to validate the ARI in preschoolers. Two samples were included: a school-based sample (N = 487, mean age = 57.80 ± 7.23 months, 52.8% male) and a clinical sample of children with Attention Deficit Hyperactivity Disorder (ADHD; N = 153, mean age = 60.5 ± 7.6 months, 83.7% males). Confirmatory factor analysis assessed ARI unidimensionality. ARI criterion validity was tested through comparison to other scales measuring irritability, related constructs, and other aspects of psychopathology. Test–retest reliability was assessed in the school-based sample. Analyses confirmed a single-factor structure and good internal consistency. The ARI showed stronger correlations with irritability measures than with measures of other constructs. In the clinical sample, ADHD children with comorbid disruptive behavior disorders had higher ARI scores than those without this comorbidity. In the school-based sample, test–retest reliability was moderate. This is the first study to demonstrate ARI validity and reliability in preschoolers. The scale performed well in both school-based and clinical samples. Having a concise and validated irritability measure for preschoolers may facilitate both clinical assessment and research on early irritability.</t>
+  </si>
+  <si>
+    <t>Assessing beliefs about emotion generation and change: The conceptualisation, development, and validation of the Cognitive Mediation Beliefs Questionnaire (CMBQ)</t>
+  </si>
+  <si>
+    <t>Martin J. Turner, Andrew G. Wood, Daniel Boatwright, Nanaki Chadha, Jennifer K. Jones, Richard Bennett</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/10503307.2020.1871524</t>
+  </si>
+  <si>
+    <t>Psychotherapy Research</t>
+  </si>
+  <si>
+    <t>The ability to regulate emotions is important for human function and health. That emotion regulation can be achieved through cognitive change is predicated on the notion of cognitive mediation. However, the extent to which individuals believe that their emotions are cognitively mediated (C–M), or in contrast, that their emotions occur via stimulus-response (S-R), is underexplored, and whether C–M and S-R beliefs shape emotion reactivity is not yet known. Research that addresses these empirical needs could inform emotion regulation interventions such as cognitive behavioural therapies (CBTs). The current paper reports the development and initial validity testing of the cognitive mediation beliefs questionnaire (CMBQ). Five studies report the factor structure, the construct and criterion validity, and the test-retest reliability of the CMBQ. The CMBQ was found to have a correlated two-factor structure (C–M change beliefs, and S-R generation beliefs). Higher C–M change beliefs and lower S-R generation beliefs were related to greater emotion regulation, greater thought control ability, higher positive mental health, and lower emotion reactivity. The CMBQ also demonstrated acceptable test-retest reliability. Initial testing indicates that the CMBQ is a valid and reliable questionnaire for psychometric use in adult populations, including those with a diagnosed mental health condition.</t>
+  </si>
+  <si>
+    <t>Phasic Versus Tonic Irritability: Differential Associations With Attention-Deficit/Hyperactivity Disorder Symptoms</t>
+  </si>
+  <si>
+    <t>Elise M. Cardinale, Gabrielle F. Freitag, Melissa A. Brotman, Daniel S. Pine, Ellen Leibenluft, Katharina Kircanski</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jaac.2020.11.022</t>
+  </si>
+  <si>
+    <t>Objective
+Irritability is a multifaceted construct in pediatric psychopathology. It has been conceptualized as having a ‘phasic’ dimension and a ‘tonic’ dimension. Disruptive mood dysregulation disorder (DMDD) is defined by the presence of both dimensions. Severe irritability, or DMDD, is highly comorbid with attention-deficit/hyperactivity disorder (ADHD). However, it is unknown whether the presence of ADHD modulates the expression of phasic and tonic irritability.
+Method
+A data-driven, latent variable approach was used to examine irritability and ADHD symptoms in a transdiagnostic pediatric sample (N=489) with primary DMDD, ADHD, subclinical irritability symptoms, or no diagnosis. Using latent profile analyses (LPA), we identified four classes: high levels of both irritability and ADHD symptoms, high levels of irritability and moderate levels of ADHD symptoms, moderate levels of irritability and high levels of ADHD symptoms, and low levels of both irritability and ADHD symptoms. Confirmatory factor analysis operationalized phasic irritability and tonic irritability.
+Results
+As expected, the two latent classes characterized by high overall irritability exhibited the highest levels of both phasic and tonic irritability. However, between these two high irritability classes, highly comorbid ADHD symptoms were associated with significantly greater phasic irritability than were moderately comorbid ADHD symptoms. In contrast, the two high irritability groups did not differ on levels of tonic irritability.
+Conclusion
+These findings suggest that phasic, but not tonic, irritability has a significant association with ADHD symptoms, and that phasic and tonic might be distinct, though highly related, irritability dimensions. Future research should investigate potential mechanisms underlying this differential association.</t>
+  </si>
+  <si>
+    <t>Neural mechanisms of reward processing in adolescent irritability</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/dev.22090</t>
+  </si>
+  <si>
+    <t>Maria Kryza‐Lacombe, Brianna Hernandez, Cassidy Owen, Richard C. Reynolds, Lauren S. Wakschlag, Lea R. Dougherty, Jillian L. Wiggins</t>
+  </si>
+  <si>
+    <t>Irritability is impairing and prevalent across pediatric psychiatric disorders and typical development, yet its neural mechanisms are largely unknown. This study evaluated the relation between adolescent irritability and reward‐related brain function as a candidate neural mechanism. Adolescents from intervention‐seeking families in the community (N = 52; mean age = 13.80, SD = 1.94) completed a monetary incentive delay task to assess reward anticipation and feedback (reward receipt and omission) during fMRI acquisition. Whole‐brain analyses, controlling for age, examined brain activation and striatal and amygdala connectivity in relation to irritability. Irritability was measured using the parent‐ and youth‐reported Affective Reactivity Index. Irritability was associated with altered reward processing‐related activation and connectivity in multiple networks during reward anticipation and feedback, including increased striatal activation and altered ventral striatum connectivity with prefrontal areas. Our findings suggest that irritability is associated with altered neural patterns during reward processing and that aberrant prefrontal cortex‐mediated top‐down control may be related to irritability. These findings inform our understanding of the etiology of youth irritability and the development of mechanism‐based interventions.</t>
+  </si>
+  <si>
+    <t>Developmental Psychobiology</t>
+  </si>
+  <si>
+    <t>Functional connectivity during frustration: a preliminary study of predictive modeling of irritability in youth</t>
+  </si>
+  <si>
+    <t>Dustin Scheinost, Javid Dadashkarimi, Emily S. Finn, Caroline G. Wambach, Caroline MacGillivray, Alexandra L. Roule, Tara A. Niendam, Daniel S. Pine, Melissa A. Brotman, Ellen Leibenluft, Wan-Ling Tseng</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41386-020-00954-8</t>
+  </si>
+  <si>
+    <t>Irritability cuts across many pediatric disorders and is a common presenting complaint in child psychiatry; however, its neural mechanisms remain unclear. One core pathophysiological deficit of irritability is aberrant responses to frustrative nonreward. Here, we conducted a preliminary fMRI study to examine the ability of functional connectivity during frustrative nonreward to predict irritability in a transdiagnostic sample. This study included 69 youths (mean age = 14.55 years) with varying levels of irritability across diagnostic groups: disruptive mood dysregulation disorder (n = 20), attention-deficit/hyperactivity disorder (n = 14), anxiety disorder (n = 12), and controls (n = 23). During fMRI, participants completed a frustrating cognitive flexibility task. Frustration was evoked by manipulating task difficulty such that, on trials requiring cognitive flexibility, “frustration” blocks had a 50% error rate and some rigged feedback, while “nonfrustration” blocks had a 10% error rate. Frustration and nonfrustration blocks were randomly interspersed. Child and parent reports of the affective reactivity index were used as dimensional measures of irritability. Connectome-based predictive modeling, a machine learning approach, with tenfold cross-validation was conducted to identify networks predicting irritability. Connectivity during frustration (but not nonfrustration) blocks predicted child-reported irritability (ρ = 0.24, root mean square error = 2.02, p = 0.03, permutation testing, 1000 iterations, one-tailed). Results were adjusted for age, sex, medications, motion, ADHD, and anxiety symptoms. The predictive networks of irritability were primarily within motor-sensory networks; among motor-sensory, subcortical, and salience networks; and between these networks and frontoparietal and medial frontal networks. This study provides preliminary evidence that individual differences in irritability may be associated with functional connectivity during frustration, a phenotype-relevant state.</t>
   </si>
 </sst>
 </file>
@@ -3907,11 +4001,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I195"/>
+  <dimension ref="A1:I201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F161" sqref="F161"/>
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G202" sqref="G202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4893,7 +4987,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>143</v>
       </c>
@@ -5128,7 +5222,7 @@
       </c>
       <c r="I45" s="14"/>
     </row>
-    <row r="46" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>175</v>
       </c>
@@ -5911,7 +6005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>280</v>
       </c>
@@ -7487,7 +7581,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>495</v>
       </c>
@@ -7539,7 +7633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>502</v>
       </c>
@@ -8825,7 +8919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A189" s="4" t="s">
         <v>680</v>
       </c>
@@ -9007,6 +9101,162 @@
         <v>8</v>
       </c>
       <c r="H195" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A196" s="4" t="s">
+        <v>900</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D196" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E196" s="15" t="s">
+        <v>902</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="G196" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H196" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A197" s="4" t="s">
+        <v>904</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D197" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E197" s="15" t="s">
+        <v>905</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="G197" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H197" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A198" s="4" t="s">
+        <v>908</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="D198" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E198" s="15" t="s">
+        <v>910</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="G198" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H198" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A199" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D199" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E199" s="15" t="s">
+        <v>915</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="G199" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H199" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A200" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="D200" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E200" s="15" t="s">
+        <v>918</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="G200" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H200" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A201" s="4" t="s">
+        <v>922</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D201" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E201" s="15" t="s">
+        <v>924</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H201" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -9390,8 +9640,20 @@
     <hyperlink ref="E159" r:id="rId373" xr:uid="{A3BB74B5-9CF5-40B2-9B96-10521AC9A3F2}"/>
     <hyperlink ref="E160" r:id="rId374" xr:uid="{A684A94C-E6A1-45B5-B206-BC12AFFB5542}"/>
     <hyperlink ref="E161" r:id="rId375" xr:uid="{842530ED-BF47-46DB-9200-43CDFB159922}"/>
+    <hyperlink ref="A196" r:id="rId376" xr:uid="{E79013DA-48FA-4771-904F-D373789A8A5C}"/>
+    <hyperlink ref="E196" r:id="rId377" xr:uid="{9CDAA8A0-5110-4F75-8486-173F384A88AF}"/>
+    <hyperlink ref="E197" r:id="rId378" xr:uid="{0BBA0ECC-25FE-4FD0-9121-70E85186D588}"/>
+    <hyperlink ref="A197" r:id="rId379" xr:uid="{716CE3EB-5916-41CD-BF9D-C289C16C02AA}"/>
+    <hyperlink ref="A198" r:id="rId380" xr:uid="{009E9533-8DDF-4021-91FF-2AAF9A9EA1B9}"/>
+    <hyperlink ref="E198" r:id="rId381" xr:uid="{A27C88FA-68F9-46EC-A489-EB1E3BF1552F}"/>
+    <hyperlink ref="A199" r:id="rId382" xr:uid="{D1263A5E-1E89-461D-83B4-577B3890CE0D}"/>
+    <hyperlink ref="E199" r:id="rId383" xr:uid="{A529904D-D0CD-40BA-9799-98500D32F478}"/>
+    <hyperlink ref="A200" r:id="rId384" xr:uid="{8527E613-8507-48B8-B263-EB63C55285E8}"/>
+    <hyperlink ref="E200" r:id="rId385" xr:uid="{D7FB6EF4-E5C9-472D-9D23-49ABD913002B}"/>
+    <hyperlink ref="E201" r:id="rId386" xr:uid="{7D21256E-2206-4B2B-8EF4-CE75068E0400}"/>
+    <hyperlink ref="A201" r:id="rId387" xr:uid="{F0A1E49A-E31D-4946-BE3E-1AE19D96CD2A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId376"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId388"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added and sorted all papers that cite ARI from the past month
</commit_message>
<xml_diff>
--- a/All ARI Papers/Affective_Reactivity_Index_Papers.xlsx
+++ b/All ARI Papers/Affective_Reactivity_Index_Papers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\string-mbd\RA Instruction Manuals\Lily Eisner\Research\ARI\ARI-Papers\All ARI Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBB93A3-D844-4559-BCA8-4FE26F0FFF1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EFBA03-C166-4803-9DBF-0F7EE61472E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="730" windowWidth="14490" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="970" windowWidth="17370" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="936">
   <si>
     <t>Authors</t>
   </si>
@@ -3562,6 +3562,36 @@
   </si>
   <si>
     <t>Irritability cuts across many pediatric disorders and is a common presenting complaint in child psychiatry; however, its neural mechanisms remain unclear. One core pathophysiological deficit of irritability is aberrant responses to frustrative nonreward. Here, we conducted a preliminary fMRI study to examine the ability of functional connectivity during frustrative nonreward to predict irritability in a transdiagnostic sample. This study included 69 youths (mean age = 14.55 years) with varying levels of irritability across diagnostic groups: disruptive mood dysregulation disorder (n = 20), attention-deficit/hyperactivity disorder (n = 14), anxiety disorder (n = 12), and controls (n = 23). During fMRI, participants completed a frustrating cognitive flexibility task. Frustration was evoked by manipulating task difficulty such that, on trials requiring cognitive flexibility, “frustration” blocks had a 50% error rate and some rigged feedback, while “nonfrustration” blocks had a 10% error rate. Frustration and nonfrustration blocks were randomly interspersed. Child and parent reports of the affective reactivity index were used as dimensional measures of irritability. Connectome-based predictive modeling, a machine learning approach, with tenfold cross-validation was conducted to identify networks predicting irritability. Connectivity during frustration (but not nonfrustration) blocks predicted child-reported irritability (ρ = 0.24, root mean square error = 2.02, p = 0.03, permutation testing, 1000 iterations, one-tailed). Results were adjusted for age, sex, medications, motion, ADHD, and anxiety symptoms. The predictive networks of irritability were primarily within motor-sensory networks; among motor-sensory, subcortical, and salience networks; and between these networks and frontoparietal and medial frontal networks. This study provides preliminary evidence that individual differences in irritability may be associated with functional connectivity during frustration, a phenotype-relevant state.</t>
+  </si>
+  <si>
+    <t>Understanding Phasic Irritability: Anger and Distress in Children’s Temper Outbursts</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10578-021-01126-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child Psychiatry &amp; Human Development </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emily Hirsch, Kaley Davis, Zihuan Cao, Amy Krain Roy </t>
+  </si>
+  <si>
+    <t>Pediatric irritability can be highly impairing and is implicated in adverse outcomes. The phasic component, characterized by temper outbursts, is a frequent impetus to seek treatment. This study tested whether a previously described anger-distress model of tantrums applies to an outpatient sample of school-age children with clinically impairing temper outbursts (TO; 5.0–9.9 years; N = 86), and examined the clinical relevance of resulting factors through associations with measures of psychopathology, and differences between children with TO and two groups without: children with ADHD (n = 60) and healthy controls (n = 45). Factor analyses established a three-factor model: High Anger, Low Anger, Distress. These factors had unique associations with measures of irritability, externalizing problems, and internalizing problems in the TO group. Additionally, an interaction between groups and outburst factors emerged. Results provide evidence for the presence and clinical utility of the anger-distress model in children’s outbursts and suggest avenues for future pediatric irritability research.</t>
+  </si>
+  <si>
+    <t>The Use of Standard Parenting Management Training in Addressing Disruptive Mood Dysregulation Disorder: A Pilot Study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gary Byrne, Graham Connon </t>
+  </si>
+  <si>
+    <t>Journal of Contemporary Psychotherapy</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10879-021-09489-5</t>
+  </si>
+  <si>
+    <t>Parent management training has demonstrated effectiveness in the treatment of child behavioural issues and associated conduct difficulties. Anger, aggression, and irritability are common symptoms amongst children presenting with disruptive mood dysregulation disorder. Currently, there are no well-established evidence-based interventions for children presenting with symptoms of disruptive mood dysregulation disorder. This pilot study aims to assess if a standard, well-established, parent management training program (group Triple P) may be effective in addressing disruptive mood dysregulation disorder symptoms. Thirteen parents of children who presented with disruptive mood dysregulation disorder or subthreshold symptoms completed the Triple P behavioural management program (Level 4). Post-treatment, parents reported no significant change on childhood irritability. However, parents noted significant improvement on child overt aggression, behavioural difficulties and an increase in child pro-social behaviours. Despite the many limitations inherent in this pilot study, results suggest that standard parent management training may be useful in addressing overt aggression but not irritability.</t>
   </si>
 </sst>
 </file>
@@ -4001,11 +4031,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I201"/>
+  <dimension ref="A1:I203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G202" sqref="G202"/>
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D204" sqref="D204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9026,7 +9056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A193" s="4" t="s">
         <v>698</v>
       </c>
@@ -9052,7 +9082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A194" s="4" t="s">
         <v>701</v>
       </c>
@@ -9078,7 +9108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" s="4" t="s">
         <v>705</v>
       </c>
@@ -9104,7 +9134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A196" s="4" t="s">
         <v>900</v>
       </c>
@@ -9130,7 +9160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A197" s="4" t="s">
         <v>904</v>
       </c>
@@ -9156,7 +9186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="4" t="s">
         <v>908</v>
       </c>
@@ -9182,7 +9212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A199" s="4" t="s">
         <v>913</v>
       </c>
@@ -9208,7 +9238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="4" t="s">
         <v>917</v>
       </c>
@@ -9234,7 +9264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A201" s="4" t="s">
         <v>922</v>
       </c>
@@ -9258,6 +9288,61 @@
       </c>
       <c r="H201" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="48.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A202" s="4" t="s">
+        <v>926</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="D202" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E202" s="15" t="s">
+        <v>927</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="G202" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H202" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="I202" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A203" s="4" t="s">
+        <v>931</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="D203" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E203" s="15" t="s">
+        <v>934</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H203" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -9652,8 +9737,12 @@
     <hyperlink ref="E200" r:id="rId385" xr:uid="{D7FB6EF4-E5C9-472D-9D23-49ABD913002B}"/>
     <hyperlink ref="E201" r:id="rId386" xr:uid="{7D21256E-2206-4B2B-8EF4-CE75068E0400}"/>
     <hyperlink ref="A201" r:id="rId387" xr:uid="{F0A1E49A-E31D-4946-BE3E-1AE19D96CD2A}"/>
+    <hyperlink ref="A202" r:id="rId388" xr:uid="{3FE531B3-F0DE-4342-A134-73D9D9DC7A81}"/>
+    <hyperlink ref="E202" r:id="rId389" xr:uid="{9D217C43-8A50-4255-B857-A66D18ED6489}"/>
+    <hyperlink ref="E203" r:id="rId390" xr:uid="{7A43D4E4-E73D-4E4F-A730-CDEDB891179B}"/>
+    <hyperlink ref="A203" r:id="rId391" xr:uid="{CAEF9400-8900-4325-A280-828F100D8EC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId388"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId392"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Papers that Reference the ARI from March 2021 - June 2021
</commit_message>
<xml_diff>
--- a/All ARI Papers/Affective_Reactivity_Index_Papers.xlsx
+++ b/All ARI Papers/Affective_Reactivity_Index_Papers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\string-mbd\RA Instruction Manuals\Lily Eisner\Research\ARI\ARI-Papers\All ARI Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EFBA03-C166-4803-9DBF-0F7EE61472E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7364D5-6A1E-4399-96C3-B2F7E65EC4AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="970" windowWidth="17370" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5790" yWindow="470" windowWidth="13200" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="998">
   <si>
     <t>Authors</t>
   </si>
@@ -3592,6 +3592,520 @@
   </si>
   <si>
     <t>Parent management training has demonstrated effectiveness in the treatment of child behavioural issues and associated conduct difficulties. Anger, aggression, and irritability are common symptoms amongst children presenting with disruptive mood dysregulation disorder. Currently, there are no well-established evidence-based interventions for children presenting with symptoms of disruptive mood dysregulation disorder. This pilot study aims to assess if a standard, well-established, parent management training program (group Triple P) may be effective in addressing disruptive mood dysregulation disorder symptoms. Thirteen parents of children who presented with disruptive mood dysregulation disorder or subthreshold symptoms completed the Triple P behavioural management program (Level 4). Post-treatment, parents reported no significant change on childhood irritability. However, parents noted significant improvement on child overt aggression, behavioural difficulties and an increase in child pro-social behaviours. Despite the many limitations inherent in this pilot study, results suggest that standard parent management training may be useful in addressing overt aggression but not irritability.</t>
+  </si>
+  <si>
+    <t>Measurement of Dysregulation in Children and Adolescents</t>
+  </si>
+  <si>
+    <t>Robert R. Althoff, Merelise Ametti</t>
+  </si>
+  <si>
+    <t>Child and Adolescent Psychiatric Clinics of North America</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.chc.2020.10.004</t>
+  </si>
+  <si>
+    <t>KEYWORDS
+_x0001_ Review _x0001_ Behavior rating scale _x0001_ Interview, psychological _x0001_ Aggression _x0001_ Irritability
+_x0001_ Emotional regulation _x0001_ Executive function _x0001_ Child
+KEY POINTS
+_x0001_ There are numerous instruments available for assessing dysregulation during childhood
+and adolescence, including rating scales, clinical interviews, and observational measures;
+however, no gold standard exists.
+_x0001_ A few measures broadly assess challenges with self-regulation, whereas most focus on
+specific aspects of emotion dysregulation, such as aggression, outbursts, or irritability.
+_x0001_ To thoroughly assess emotion dysregulation, it is recommended that future studies
+include measures of broad psychological functioning, chronic mood regulation problems,
+and outbursts.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.chc.2020.10.013</t>
+  </si>
+  <si>
+    <t>Jennifer Keluskar, Debra Reicher, Amanda Gorecki, Carla Mazefsky, Judith A. Crowell</t>
+  </si>
+  <si>
+    <t>Autism spectrum disorder (ASD) is characterized by 2 broad domains of impairment:
+(1) “Persistent deficits in social communication and social interactions across multiple
+contexts.” and (2) “restrictive, repetitive patterns of behavior, interests, or activities.2
+” Although irritability, tantrums, and self-injurious behaviors are not core symptoms, they cause considerable distress and impairment and add to the burden for
+people with ASD. Understanding the rates of such problems in children with ASD is
+complicated by the varied terminology used to identify the important symptoms and
+behaviors (see Daniel F. Connor and Leonard A. Doerfler’s article, “The Many Faces
+(and Names) of Mood Dysregulation,” elsewhere in this issue; and Lauren Spring
+and Gabrielle A. Carlson’s article, “The Phenomenology of Outbursts,” elsewhere in
+this issue). Thus, irritability, which has multiple definitions but generally refers to a propensity toward anger, has been co-opted by the Food and Drug Administration as a
+target behavior worthy of treatment.
+Irritability is a consequence of poor emotion regulation (ER). Results of irritability and
+emotion dysregulation (ED) include impulsive aggression, tantrums, outbursts, agitation, and sometimes self-injurious behavior. Rates of ED in children with autism, when
+systematically ascertained, range from 50% to 80% (Table 1).</t>
+  </si>
+  <si>
+    <t>Understanding, Assessing, and Intervening with Emotion Dysregulation in Autism Spectrum Disorder: A Developmental Perspective</t>
+  </si>
+  <si>
+    <t>Across-subjects multiple baseline trial of exposure-based cognitive-behavioral therapy for severe irritability: a study protocol</t>
+  </si>
+  <si>
+    <t>https://dx.doi.org/10.1136%2Fbmjopen-2020-039169</t>
+  </si>
+  <si>
+    <t>Reut Naim, Katharina Kircanski, Andrea Gold,  Ramaris E German, Mollie Davis, Samantha Perlstein, Michal Clayton, Olga Revzina, and Melissa A Brotman</t>
+  </si>
+  <si>
+    <t>Introduction Irritability is defined as a tendency towards anger in response to frustration. Clinically, impairing irritability is a significant public health problem. There is a need for mechanism-based psychotherapies targeting severe irritability as it manifests in the context of disruptive mood dysregulation disorder (DMDD). This study protocol describes a randomised multiple baseline design testing the preliminary efficacy of a new treatment, exposure-based cognitive-behavioral therapy for severe irritability in youth, which also integrates components of parent management training. We will investigate associations of this intervention with primary clinical measures, as well as ecological momentary assessment measures.
+Methods and analysis Forty youth will be enrolled. Participants, aged 8–17 years, must present at least one of two core symptoms of DMDD: abnormal mood or increased reactivity to negative emotional stimuli, with severe impairment in one domain (home, school, peers) and moderate in another, or moderate impairment in at least two domains. Each participant is randomised to a 2-week, 4-week or 6-week baseline observation period, followed by 12 active treatment sessions. Clinical ratings are conducted at baseline, biweekly (clinician), weekly (parent/child) throughout treatment, post-treatment, and 3-month and 6-month follow-up (clinician). Clinician ratings on the Affective Reactivity Index and Clinical Global Impressions-Improvement scale for DMDD are our primary outcome measures. Secondary outcome measures include parent and child reports of irritability. Post hoc additional symptom measures include clinician, parent and self-ratings of depression, anxiety and overall functional impairment. Prospective, digitally based event sampling of symptoms is acquired for a week pre-treatment, mid-treatment and post-treatment. Based on our pathophysiological model of irritability implicating frustrative non-reward, aberrant threat processing and instrumental learning, we probe these three brain-based targets using functional MRI paradigms to assess target engagement.
+Ethics and dissemination The research project and all related materials were submitted and approved by the appropriate Institutional Review Board (IRB) of the National Institute of Mental Health (NIMH).
+Trial registration numbers NCT02531893 and NCT00025935.
+http://creativecommons.org/licenses/by-nc/4.0/
+This is an open access article distributed in accordance with the Creative Commons Attribution Non Commercial (CC BY-NC 4.0) license, which permits others to distribute, remix, adapt, build upon this work non-commercially, and license their derivative works on different terms, provided the original work is properly cited, appropriate credit is given, any changes made indicated, and the use is non-commercial. See: http://creativecommons.org/licenses/by-nc/4.0/.</t>
+  </si>
+  <si>
+    <t>Deliberative Choice Strategies in Youths: Relevance to Transdiagnostic Anxiety Symptoms</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177%2F2167702621991805</t>
+  </si>
+  <si>
+    <t>Elise M. Cardinale, David Pagliaccio, Caroline Swetlitz, Hannah Grassie, Rany Abend, Vincent Costa, Bruno Averbeck, Melissa A. Brotman, Daniel S. Pine, Ellen Leibenluft, Katharina Kircanski</t>
+  </si>
+  <si>
+    <t>Clinical Psychological Science</t>
+  </si>
+  <si>
+    <t>Aberrant decision-making characterizes various pediatric psychopathologies; however, deliberative choice strategies
+have not been investigated. A transdiagnostic sample of 95 youths completed a child-friendly sequential sampling
+paradigm. Participants searched for the best offer by sampling a finite list of offers. Participants’ willingness to explore
+was measured as the number of offers sampled, and ideal task performance was modeled using a Markov decisionprocess model. As in previous findings in adults, youths explored more offers when lists were long compared with
+short, yet participants generally sampled fewer offers relative to model-estimated ideal performance. Searching deeper
+into the list was associated with choosing better price options. Analyses examining the main and interactive effects of
+transdiagnostic anxiety and irritability symptoms indicated a negative correlation between anxiety and task performance
+(p = .01, ηp
+2 = .08). Findings suggest the need for more research on exploratory decision impairments in youths with
+anxiety symptoms.</t>
+  </si>
+  <si>
+    <t>The Youth and Childhood Adversity Scale:
+A step towards developing a new measure of adversity and its severity</t>
+  </si>
+  <si>
+    <t>Background: Early adversity (EA) can contribute to the onset, manifestation, and
+course of various mental disorders. Measuring EA is still conceptually and psychometrically
+challenging due to issues such as content coverage, wording of items, scaling methods, and
+validation procedures.
+Method: To this end, we have developed a 13-item measure of EA, the Youth and
+Childhood Adversity Scale (YCAS). Beyond a dichotomous assessment of whether a set of
+adverse events have been experienced, this scale assesses an important but currently underinvestigated facet of EA: the respective severity of these events. Here, we evaluate the YCAS
+in a sample of 596 adolescent students (ages 16-19) and a second sample of 451 medical
+students (ages 18-30+). We psychometrically assessed both factor scores and sum scores of
+the YCAS.
+Results: In both samples a one-factorial solution was found for both responses to
+dichotomous items and severity items. Item loadings had a broad range, with minimum
+loadings of .1-.2 and maximum loadings of .7-.9. Irrespective of response type, this factor
+exhibited good reliability (omega total) and was associated with a range of mental health
+outcome measures, self-esteem, and childhood maltreatment. The sum score reliability
+(coefficient alpha) was acceptable and most of the associations with the validation measures
+held.
+Conclusions: The YCAS allows an efficient, reliable, and valid assessment of EA.
+The YCAS covers a reasonable breadth of events, while simultaneously being parsimonious.
+The psychometric soundness of the severity facet suggests that the assessment of adversity
+severity may be worthwhile, but needs further examination.</t>
+  </si>
+  <si>
+    <t>Pascal Schlechter, Jessica Fritz, Matthew Cassels, Sharon A.S. Neufeld, Paul O. Wilkinson</t>
+  </si>
+  <si>
+    <t>Attention bias to negative versus non-negative faces is related to negative affectivity in a transdiagnostic youth sample</t>
+  </si>
+  <si>
+    <t>Anita Harrewijn, Rany Abend, Reut Naim, Simone P. Haller, Caitlin M. Stavish, Mira A. Bajaj, Chika Matsumoto, Kelly Dombek, Elise M. Cardinale, Katharina Kircanski, Melissa A. Brotman</t>
+  </si>
+  <si>
+    <t>Journal of Psychiatric Research</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jpsychires.2021.04.036</t>
+  </si>
+  <si>
+    <t>This study identified a shared pathophysiological mechanism of pediatric anxiety and irritability. Clinically, anxiety and irritability are common, co-occurring problems, both characterized by high-arousal negative affective states. Behaviorally, anxiety and irritability are associated with aberrant threat processing. To build on these findings, we examined eye-tracking measures of attention bias in relation to the unique and shared features of anxiety and irritability in a transdiagnostic sample of youth (n = 97, 58% female, Mage = 13.03, SDage = 2.82). We measured attention bias to negative versus non-negative emotional faces during a passive viewing task. We employed bifactor analysis to parse the unique and shared variance of anxiety and irritability symptoms from self- and parent-report questionnaires. Negative affectivity is the derived latent factor reflecting shared variance of anxiety and irritability. We found that higher negative affectivity was associated with looking longer at negative versus non-negative faces, reflecting a shared mechanism of anxiety and irritability. This finding suggests that modification of elevated attention to negative emotional faces may represent a common potential treatment target of anxiety and irritability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduced neural responsiveness to looming stimuli is associated with increased aggression </t>
+  </si>
+  <si>
+    <t>R James Blair, Ru Zhang, Johannah Bashford-Largo, Sahil Bajaj, Avantika Mathur, Jay Ringle, Amanda Schwartz, Jaimie Elowsky, Matthew Dobbertin, Karina S Blair, Patrick M Tyler</t>
+  </si>
+  <si>
+    <t>Social Cognitive and Affective Neuroscience</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/scan/nsab058</t>
+  </si>
+  <si>
+    <t>While neuro-cognitive work examining aggression has examined patients with conditions at increased risk for aggression or individuals self-reporting past aggression, little work has attempted to identify neuro-cognitive markers associated with observed/recorded aggression. The goal of the current study was to determine the extent to which aggression by youth in the first three months of residential care was associated with atypical responsiveness to threat stimuli. This functional MRI study involved 98 (68 male; mean age = 15.96 [sd = 1.52]) adolescents in residential care performing a looming threat task involving images of threatening and neutral human faces or animals that appeared to be either loom or recede. Level of aggression was negatively associated with responding to looming stimuli (irrespective of whether these were threatening or neutral) within regions including bilateral inferior frontal gyrus, right inferior parietal lobule, right superior/middle temporal gyrus and a region of right uncus proximal to the amygdala. These data indicate that aggression level is associated with a decrease in responsiveness to a basic threat cue-looming stimuli. Reduced threat responsiveness likely results in the individual being less able to represent the negative consequences that may result from engaging in aggression, thereby increasing the risk for aggressive episodes.</t>
+  </si>
+  <si>
+    <t>Irritability in developmental age: A narrative review of a dimension crossing paediatric psychopathology</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1177%2F00048674211011245</t>
+  </si>
+  <si>
+    <t>Maria Breda, Ignazio Ardizzone</t>
+  </si>
+  <si>
+    <t>Objective:
+Irritability is an important theme in paediatric psychiatry considering its high frequency in developmental age, its association with negative outcomes and consequently significant public health impact. Present as main or associated feature of several psychiatric diagnoses, irritability represents a challenge for clinicians who try to understand its origin and role in developmental psychopathology. In this review we try to: (1) get an overview of this dimension and its relationship with each of the main neuropsychiatric disorders in paediatric population and (2) provide a summary of currently available instruments to assess irritability in children and adolescents.
+Method:
+In this narrative review, an overview of irritability in children and adolescents is proposed focusing on selected literature.
+Results:
+Irritability as feature of many paediatric psychiatric conditions has been evaluated by many authors and included in classifications of paediatric psychiatric diseases. Framework of irritability evolved over time and dimension of irritability has been investigated using different tools and methodologies, both qualitative and quantitative. Metrics of irritability as clinical dimension are important in the diagnostic process of paediatric diseases.
+Conclusion:
+Investigating the presence of irritability in all children with related disorders is mandatory if we consider the risk for functional impairment and affective and behavioural disorders associated with high levels of irritability. Using rigid threshold in developmental age to differentiate physiological from pathological irritability could lead many children having subthreshold levels of irritability to receive no diagnosis and, consequently, no treatment where instead a dimensional approach to irritability could allow to identify prodromal phase and prevent the evolution towards clinical pathological expressions.
+Keywords Irritability, depression, disruptive mood dysregulation disorder, developmental psychopathology, transdiagnostic
+Access Options
+My Account
+Email (required): 
+Email address
+Password (required): 
+Password
+ Remember me
+Forgotten your password?
+Need to activate?
+Need Help?
+Institutional Login
+NIH LIBRARY does not have access to this content.
+If you have access to journal content via a university, library or employer, sign in here
+Access through your institution
+Need Help?
+RANZCP Member Access
+RANZCP members have access to this journal as part of their membership. Sign in using your membership username and password.
+Purchase Content
+24 hours online access to download content
+Article
+$41.50
+Add to Cart
+Subscribe to this journal
+Recommend to your library
+Need Help?
+Rent with DeepDyve
+Rent Article
+Research off-campus without worrying about access issues. Find out about Lean Library here
+References
+Achenbach, TM (1997) What is normal? What is abnormal? Developmental perspectives on behavioral and emotional problems. In: Luthar, SS, Burack, JA, Cicchetti, D, et al. (eds) Developmental Psychopathology: Perspectives on Adjustment, Risk, and Disorder. Cambridge: Cambridge University Press, pp. 93–114.
+Google Scholar
+Aebi, M, Barra, S, Bessler, C, et al. (2016) Oppositional defiant disorder dimensions and subtypes among detained male adolescent offenders. Journal of Child Psychology and Psychiatry and Allied Disciplines 57: 729–736.
+Google Scholar | Crossref | Medline
+Aebi, M, Plattner, B, Metzke, CW, et al. (2013) Parent- and self-reported dimensions of oppositionality in youth: Construct validity, concurrent validity, and the prediction of criminal outcomes in adulthood. Journal of Child Psychology and Psychiatry 54: 941–949.
+Google Scholar | Crossref | Medline
+Althoff, RR, Kuny-Slock, AV, Verhulst, FC, et al. (2014) Classes of oppositional-defiant behavior: Concurrent and predictive validity. Journal of Child Psychology and Psychiatry and Allied Disciplines 55: 1162–1171.
+Google Scholar | Crossref | Medline
+Althoff, RR, Crehan, ET, He, J-P, et al. (2016) Disruptive mood dysregulation disorder at ages 13-18: Results from the national comorbidity survey – Adolescent supplement. Journal of Child and Adolescent Psychopharmacology 26: 107–113.
+Google Scholar | Crossref | Medline | ISI
+Ambrosini, PJ, Bennett, DS, Elia, J (2013) Attention deficit hyperactivity disorder characteristics: II. Clinical correlates of irritable mood. Journal of Affective Disorders 145: 70–76.
+Google Scholar | Crossref | Medline | ISI
+American Psychiatric Association (2013) American Psychiatric Association: Diagnostic and Statistical Manual of Mental Disorders, 5th Edition. Arlington, VA: American Psychiatric Association.
+Google Scholar | Crossref
+Axelson, D (2013) Taking disruptive mood dysregulation disorder out for a test drive. American Journal of Psychiatry 170: 136–139.
+Google Scholar | Crossref | Medline
+Axelson, D, Findling, RL, Fristad, MA, et al. (2012) Examining the proposed disruptive mood dysregulation disorder diagnosis in children in the Longitudinal Assessment of Manic Symptoms study. Journal of Clinical Psychiatry 73: 1342–1350.
+Google Scholar | Crossref | Medline | ISI
+Axelson, DA, Birmaher, B, Findling, RL, et al. (2011) Concerns regarding the inclusion of temper dysregulation disorder with dysphoria in the DSM-5. Journal of Clinical Psychiatry 72: 1257–1262.
+Google Scholar | Crossref | Medline | ISI
+Barkley, RA, Fischer, M (2010) The unique contribution of emotional impulsiveness to impairment in major life activities in hyperactive children as adults. Journal of the American Academy of Child and Adolescent Psychiatry 49: 503–513.
+Google Scholar | Crossref | Medline | ISI
+Bell, E, Malhi, GS (2020) Irritability: An inability, or an ability? Australian and New Zealand Journal of Psychiatry 54: 1232–1233.
+Google Scholar | SAGE Journals | ISI
+Blader, JC, Carlson, GA (2007) Increased rates of bipolar disorder diagnoses among U.S. child, adolescent, and adult inpatients, 1996-2004. Biological Psychiatry 62: 107–114.
+Google Scholar | Crossref | Medline | ISI
+Bolhuis, K, Lubke, GH, van der Ende, J, et al. (2017) Disentangling heterogeneity of childhood disruptive behavior problems into dimensions and subgroups. Journal of the American Academy of Child and Adolescent Psychiatry 56: 678–686.
+Google Scholar | Crossref | Medline
+Burke, JD (2012) An affective dimension within oppositional defiant disorder symptoms among boys: Personality and psychopathology outcomes into early adulthood. Journal of Child Psychology and Psychiatry 53: 1176–1183.
+Google Scholar | Crossref | Medline | ISI
+Burke, JD, Hipwell, AE, Loeber, R (2010) Dimensions of oppositional defiant disorder as predictors of depression and conduct disorder in preadolescent girls. Journal of the American Academy of Child and Adolescent Psychiatry 49: 484–492.
+Google Scholar | Crossref | Medline | ISI
+Burke, JD, Rowe, R, Boylan, K (2014) Functional outcomes of child and adolescent oppositional defiant disorder symptoms in young adult men. Journal of Child Psychology and Psychiatry and Allied Disciplines 55: 264–272.
+Google Scholar | Crossref | Medline | ISI
+Buss, AH, Durkee, A (1957) An inventory for assessing different kinds of hostility. Journal of Consulting Psychology 21: 343–349.
+Google Scholar | Crossref | Medline
+Caprara, GV, Cinanni, V, D’Imperio, G, et al. (1985) Indicators of impulsive aggression: Present status of research on irritability and emotional susceptibility scales. Personality and Individual Differences 6: 665–674.
+Google Scholar | Crossref | ISI
+Carlson, GA, Danzig, AP, Dougherty, LR, et al. (2016) Loss of temper and irritability: The relationship to tantrums in a community and clinical sample. Journal of Child and Adolescent Psychopharmacology 26: 114–122.
+Google Scholar | Crossref | Medline | ISI
+Conner, KR, Meldrum, S, Wieczorek, WF, et al. (2004) The association of irritability and impulsivity with suicidal ideation among 15- to 20-year-old males. Suicide and Life-Threatening Behavior 34: 363–373.
+Google Scholar | Crossref | Medline
+Copeland, WE, Shanahan, L, Costello, EJ, et al. (2009) Childhood and adolescent psychiatric disorders as predictors of young adult disorders. Archives of General Psychiatry 66: 764–772.
+Google Scholar | Crossref | Medline
+Copeland, WE, Angold, A, Costello, EJ, et al. (2013) Prevalence, comorbidity, and correlates of DSM-5 proposed disruptive mood dysregulation disorder. American Journal of Psychiatry 170: 173–179.
+Google Scholar | Crossref | Medline | ISI
+Dougherty, LR, Smith, VC, Bufferd, SJ, et al. (2014) DSM-5 disruptive mood dysregulation disorder: Correlates and predictors in young children. Psychological Medicine 44: 2339–2350.
+Google Scholar | Crossref | Medline | ISI
+Dougherty, LR, Smith, VC, Bufferd, SJ, et al. (2015) Preschool irritability predicts child psychopathology, functional impairment, and service use at age nine. Journal of Child Psychology and Psychiatry 56: 999–1007.
+Google Scholar | Crossref | Medline
+Drabick, DAG, Gadow, KD (2012) Deconstructing oppositional defiant disorder: Clinic-based evidence for an anger/irritability phenotype. Journal of the American Academy of Child and Adolescent Psychiatry 51: 384–393.
+Google Scholar | Crossref | Medline | ISI
+Egger, HL, Angold, A (2006) Common emotional and behavioral disorders in preschool children: Presentation, nosology, and epidemiology. Journal of Child Psychology and Psychiatry and Allied Disciplines 7: 313–337.
+Google Scholar | Crossref
+Evans, SC, Burke, JD, Roberts, MC, et al. (2017) Irritability in child and adolescent psychopathology: An integrative review for ICD-11. Clinical Psychology Review 53: 29–45.
+Google Scholar | Crossref | Medline | ISI
+Eyre, O, Langley, K, Stringaris, A, et al. (2017) Irritability in ADHD: Associations with depression liability. Journal of Affective Disorders 215: 281–287.
+Google Scholar | Crossref | Medline
+Ezpeleta, L, Granero, R, de la Osa, N, et al. (2012) Dimensions of oppositional defiant disorder in 3-year-old preschoolers. Journal of Child Psychology and Psychiatry and Allied Disciplines 44: 115–128.
+Google Scholar
+Ezpeleta, L, Granero, R, de la Osa, N, et al. (2016) Trajectories of oppositional defiant disorder irritability symptoms in preschool children. Journal of Abnormal Child Psychology 44: 115–128.
+Google Scholar | Crossref | Medline
+Fernández de la Cruz, L, Simonoff, E, McGough, JJ, et al. (2015) Treatment of children with attention-deficit/hyperactivity disorder (ADHD) and irritability: Results from the multimodal treatment study of children with ADHD (MTA). Journal of the American Academy of Child and Adolescent Psychiatry 54: 62–70.
+Google Scholar
+Frazier, EA, Liu, RT, Massing-Schaffer, M, et al. (2016) Adolescent but not parent report of irritability is related to suicidal ideation in psychiatrically hospitalized adolescents. Archives of Suicide Research 20: 280–289.
+Google Scholar | Crossref | Medline
+Haller, SP, Kircanski, K, Stringaris, A, et al. (2020) The clinician affective reactivity index: Validity and reliability of a clinician-rated assessment of irritability. Behavior Therapy. Association for Behavioral and Cognitive Therapies 51: 283–293.
+Google Scholar
+Karalunas, SL, Fair, D, Musser, ED, et al. (2014) Subtyping attention-deficit/hyperactivity disorder using temperament dimensions: Toward biologically based nosologic criteria. JAMA Psychiatry 71: 1015–1024.
+Google Scholar | Crossref | Medline | ISI
+Karalunas, SL, Gustafsson, HC, Fair, D, et al. (2019) Do we need an irritable subtype of ADHD? Replication and extension of a promising temperament profile approach to ADHD subtyping. Psychological Assessment 31: 236–247.
+Google Scholar | Crossref | Medline
+Kazdin, AE, Rodgers, A, Colbus, D, et al. (1987) Children’s hostility inventory: Measurement of aggression and hostility in psychiatric inpatient children. Journal of Clinical Child Psychology 16: 320–328.
+Google Scholar | Crossref
+Kendler, KS (1996) Major depression and generalised anxiety disorder. British Journal of Psychiatry 168: 68–75.
+Google Scholar | Crossref | Medline | ISI
+Kolko, DJ, Pardini, DA (2010) ODD dimensions, ADHD, and callous-unemotional traits as predictors of treatment response in children with disruptive behavior disorders. Journal of Abnormal Psychology 119: 713–725.
+Google Scholar | Crossref | Medline | ISI
+Krieger, FV, Stringaris, A (2013) Bipolar disorder and disruptive mood dysregulation in children and adolescents: Assessment, diagnosis and treatment. Evidence-Based Mental Health 16: 93–94.
+Google Scholar | Crossref | Medline
+Kuny, AV, Althoff, RR, Copeland, W, et al. (2013) Separating the domains of oppositional behavior: Comparing latent models of the Conners’ oppositional subscale. Journal of the American Academy of Child and Adolescent Psychiatry 52: 172–183.
+Google Scholar | Crossref | Medline
+Lavigne, JV, Gouze, KR, Bryant, FB, et al. (2014) Dimensions of oppositional defiant disorder in young children: Heterotypic continuity with anxiety and depression. Journal of Abnormal Child Psychology 42: 937–951.
+Google Scholar | Crossref | Medline
+Leadbeater, BJ, Homel, J (2015) Irritable and defiant sub-dimensions of ODD: Their stability and prediction of internalizing symptoms and conduct problems from adolescence to young adulthood. Journal of Abnormal Child Psychology 43: 407–421.
+Google Scholar | Crossref | Medline | ISI
+Leibenluft, E (2011) Severe mood dysregulation, irritability, and the diagnostic boundaries of bipolar disorder in youths. American Journal of Psychiatry 168: 129–142.
+Google Scholar | Crossref | Medline | ISI
+Leibenluft, E, Charney, DS, Towbin, KE, et al. (2003) Defining clinical phenotypes of juvenile mania. American Journal of Psychiatry 160: 430–437.
+Google Scholar | Crossref | Medline | ISI
+Leibenluft, E, Cohen, P, Gorrindo, T, et al. (2006) Chronic versus episodic irritability in youth: A community-based, longitudinal study of clinical and diagnostic associations. Journal of Child and Adolescent Psychopharmacology 16: 456–466.
+Google Scholar | Crossref | Medline | ISI
+Liu, L, Chen, W, Vitoratou, S, et al. (2019) Is emotional lability distinct from ‘angry/irritable mood’, ‘negative affect’, or other subdimensions of oppositional defiant disorder in children with ADHD? Journal of Attention Disorders 23: 859–868.
+Google Scholar | SAGE Journals | ISI
+Maire, J, Galera, C, Bioulac, S, et al. (2020) Emotional lability and irritability have specific associations with symptomatology in children with attention deficit hyperactivity disorder. Psychiatry Research 285: 112789.
+Google Scholar | Crossref | Medline
+Margulies, DM, Weintraub, S, Basile, J, et al. (2012) Will disruptive mood dysregulation disorder reduce false diagnosis of bipolar disorder in children? Bipolar Disorder 14: 488–496.
+Google Scholar | Crossref | Medline | ISI
+Markon, KE, Krueger, RF, Watson, D (2005) Delineating the structure of normal and abnormal personality: An integrative hierarchical approach. Journal of Personality and Social Psychology 88: 139–157.
+Google Scholar | Crossref | Medline | ISI
+Masi, G, Millepiedi, S, Mucci, M, et al. (2003) Phenomenology and comorbidity of dysthymic disorder in 100 consecutively referred children and adolescents: Beyond DSM-IV. Canadian Journal of Psychiatry 48: 99–105.
+Google Scholar | SAGE Journals | ISI
+Mayes, SD, Mathiowetz, C, Kokotovich, C, et al. (2015) Stability of disruptive mood dysregulation disorder symptoms (irritable-angry mood and temper outbursts) throughout childhood and adolescence in a general population sample. Journal of Abnormal Child Psychology 43: 1543–1549.
+Google Scholar | Crossref | Medline | ISI
+Merwood, A, Chen, W, Rijsdijk, F, et al. (2014) Genetic associations between the symptoms of attention-deficit/ hyperactivity disorder and emotional lability in child and adolescent twins. Journal of the American Academy of Child and Adolescent Psychiatry 53: 209.e4–220.e4.
+Google Scholar | Medline
+Mikita, N, Stringaris, A (2013) Mood dysregulation. European Child and Adolescent Psychiatry 22: S11–S16.
+Google Scholar | Crossref | Medline
+Mikolajewski, AJ, Taylor, J, Iacono, WG (2017) Oppositional defiant disorder dimensions: Genetic influences and risk for later psychopathology. Journal of Child Psychology and Psychiatry and Allied Disciplines 58: 702–710.
+Google Scholar | Crossref | Medline
+Moffitt, TE (1993) Adolescence-limited and life-course-persistent antisocial behavior: A developmental taxonomy. Psychological Review 100: 674–701.
+Google Scholar | Crossref | Medline | ISI
+Moore, CC, Hubbard, JA, Bookhout, MK, et al. (2019) Relations between reactive and proactive aggression and daily emotions in adolescents. Journal of Abnormal Child Psychology 47: 1495–1507.
+Google Scholar | Crossref | Medline
+Moreno, C, Laje, G, Blanco, C, et al. (2007) National trends in the outpatient diagnosis and treatment of bipolar disorder in youth. Archives of General Psychiatry 64: 1032–1039.
+Google Scholar | Crossref | Medline
+Mulraney, M, Schilpzand, EJ, Hazell, P, et al. (2016) Comorbidity and correlates of disruptive mood dysregulation disorder in 6–8-year-old children with ADHD. European Child and Adolescent Psychiatry 25: 321–330.
+Google Scholar | Crossref | Medline | ISI
+Muratori, P, Pisano, S, Milone, A, et al. (2017) Is emotional dysregulation a risk indicator for auto-aggression behaviors in adolescents with oppositional defiant disorder? Journal of Affective Disorders 208: 110–112.
+Google Scholar | Crossref | Medline
+Orri, M, Galera, C, Turecki, G, et al. (2019) Pathways of association between childhood irritability and adolescent suicidality. Journal of the American Academy of Child and Adolescent Psychiatry 58: 99–107.
+Google Scholar | Crossref | Medline
+Parens, E, Johnston, J (2010) Controversies concerning the diagnosis and treatment of bipolar disorder in children. Child and Adolescent Psychiatry and Mental Health 4: 9.
+Google Scholar | Crossref | Medline
+Peterson, BS, Zhang, H, Santa Lucia, R, et al. (1996) Risk factors for presenting problems in child psychiatric emergencies. Journal of the American Academy of Child and Adolescent Psychiatry 35: 1162–1173.
+Google Scholar | Crossref | Medline
+Pickles, A, Aglan, A, Collishaw, S, et al. (2010) Predictors of suicidality across the life span: The Isle of Wight study. Psychological Medicine 40: 1453–1466.
+Google Scholar | Crossref | Medline | ISI
+Pylypow, J, Quinn, D, Duncan, D, et al. (2020) A measure of emotional regulation and irritability in children and adolescents: The clinical evaluation of emotional regulation–9. Journal of Attention Disorders 24: 2002–2011.
+Google Scholar | SAGE Journals | ISI
+Raine, A, Ishikawa, SS, Arce, E, et al. (2004) Hippocampal structural asymmetry in unsuccessful psychopaths. Biological Psychiatry 55: 185–191.
+Google Scholar | Crossref | Medline | ISI
+Raven, M, Parry, P (2012) Psychotropic marketing practices and problems: Implications for DSM-5. Journal of Nervous and Mental Disease 200: 512–516.
+Google Scholar | Crossref | Medline
+Rieffe, C, Broekhof, E, Kouwenberg, M, et al. (2016) Disentangling proactive and reactive aggression in children using self-report. European Journal of Developmental Psychology 13: 439–451.
+Google Scholar | Crossref | Medline
+Riglin, L, Eyre, O, Thapar, AK, et al. (2019) Identifying novel types of irritability using a developmental genetic approach. American Journal of Psychiatry 176: 635–642.
+Google Scholar | Crossref | Medline
+Rowe, R, Costello, EJ, Angold, A, et al. (2010) Developmental pathways in oppositional defiant disorder and conduct disorder. Journal of Abnormal Psychology 119: 726–738.
+Google Scholar | Crossref | Medline | ISI
+Roy, AK, Brotman, MA, Leibenluft, E (2019) Introduction. In: Roy, AK, Brotman, MA, Leibenluft, E (eds) Irritability in Pediatric Psychopathology. Oxford: Oxford University Press, pp. 1–10.
+Google Scholar | Crossref
+Savage, J, Verhulst, B, Copeland, W, et al. (2015) A genetically informed study of the longitudinal relation between irritability and anxious/depressed symptoms. Journal of the American Academy of Child and Adolescent Psychiatry 54: 377–384.
+Google Scholar | Crossref | Medline | ISI
+Shaw, P, Stringaris, A, Nigg, J, et al. (2014) Emotion dysregulation in attention deficit hyperactivity disorder. American Journal of Psychiatry 171: 276–293.
+Google Scholar | Crossref | Medline | ISI
+Sjöwall, D, Roth, L, Lindqvist, S, et al. (2013) Multiple deficits in ADHD: Executive dysfunction, delay aversion, reaction time variability, and emotional deficits. Journal of Child Psychology and Psychiatry and Allied Disciplines 54: 619–627.
+Google Scholar | Crossref | Medline | ISI
+Snaith, RP, Taylor, CM (1985) Irritability definition, assessment and associated factors. British Journal of Psychiatry 147: 127–136.
+Google Scholar | Crossref | Medline | ISI
+Stringaris, A, Goodman, R (2009a) Longitudinal outcome of youth oppositionality: Irritable, headstrong, and hurtful behaviors have distinctive predictions. Journal of the American Academy of Child and Adolescent Psychiatry 48: 404–412.
+Google Scholar | Crossref | Medline | ISI
+Stringaris, A, Goodman, R (2009b) Three dimensions of oppositionality in youth. Journal of Child Psychology and Psychiatry and Allied Disciplines 50: 216–223.
+Google Scholar | Crossref | Medline | ISI
+Stringaris, A, Vidal-Ribas, P (2019) Probing the irritability – Suicidality nexus. Journal of the American Academy of Child and Adolescent Psychiatry 58: 18–19.
+Google Scholar | Crossref | Medline
+Stringaris, A, Goodman, R, Ferdinando, S, et al. (2012a) The Affective Reactivity Index: A concise irritability scale for clinical and research settings. Journal of Child Psychology and Psychiatry and Allied Disciplines 53: 1109–1117.
+Google Scholar | Crossref | Medline | ISI
+Stringaris, A, Zavos, H, Leibenluft, E, et al. (2012b) Adolescent irritability: Phenotypic associations and genetic links with depressed mood. American Journal of Psychiatry 169: 47–54.
+Google Scholar | Crossref | Medline | ISI
+Tufan, E, Topal, Z, Demir, N, et al. (2016) Sociodemographic and clinical features of disruptive mood dysregulation disorder: A chart review. Journal of Child and Adolescent Psychopharmacology 26: 94–100.
+Google Scholar | Crossref | Medline | ISI
+Vidal-Ribas, P, Brotman, MA, Valdivieso, I, et al. (2016) The status of irritability in psychiatry: A conceptual and quantitative review. Journal of the American Academy of Child and Adolescent Psychiatry 55: 556–570.
+Google Scholar | Crossref | Medline | ISI
+Vitaro, F, Barker, ED, Boivin, M, et al. (2006) Do early difficult temperament and harsh parenting differentially predict reactive and proactive aggression? Journal of Abnormal Child Psychology 34: 685–695.
+Google Scholar | Crossref | Medline | ISI
+Wakschlag, LS, Briggs-Gowan, MJ, Hill, C, et al. (2008a) Observational assessment of preschool disruptive behavior, part II: Validity of the disruptive behavior diagnostic observation schedule (DB-DOS). Journal of the American Academy of Child and Adolescent Psychiatry 47: 632–641.
+Google Scholar | Crossref | Medline | ISI
+Wakschlag, LS, Choi, SW, Carter, AS, et al. (2012) Defining the developmental parameters of temper loss in early childhood: Implications for developmental psychopathology. Journal of Child Psychology and Psychiatry and Allied Disciplines 53: 1099–1108.
+Google Scholar | Crossref | Medline
+Wakschlag, LS, Estabrook, R, Petitclerc, A, et al. (2015) Clinical implications of a dimensional approach: The normal:abnormal spectrum of early irritability. Journal of the American Academy of Child and Adolescent Psychiatry 54: 626–634.
+Google Scholar | Crossref | Medline
+Wakschlag, LS, Hill, C, Carter, AS, et al. (2008b) Observational assessment of preschool disruptive behavior, part I: Reliability of the disruptive behavior diagnostic observation schedule (DB-DOS). Journal of the American Academy of Child and Adolescent Psychiatry 47: 622–631.
+Google Scholar | Crossref | Medline | ISI
+Wakschlag, LS, Krogh-Jespersen, S, Estabrook, R, et al. (2020) The early childhood irritability-related impairment interview (E-CRI): A novel method for assessing young children’s developmentally impairing irritability. Behavior Therapy 51: 670–673.
+Google Scholar | Crossref | Medline
+Whelan, YM, Leibenluft, E, Stringaris, A, et al. (2015) Pathways from maternal depressive symptoms to adolescent depressive symptoms: The unique contribution of irritability symptoms. Journal of Child Psychology and Psychiatry and Allied Disciplines 56: 1092–1100.
+Google Scholar | Crossref | Medline
+Whelan, YM, Stringaris, A, Maughan, B, et al. (2013) Developmental continuity of oppositional defiant disorder subdimensions at ages 8, 10, and 13 years and their distinct psychiatric outcomes at age 16 years. Journal of the American Academy of Child and Adolescent Psychiatry 52: 961–969.
+Google Scholar | Crossref | Medline | ISI
+Winters, DE, Fukui, S, Leibenluft, E, et al. (2018) Improvements in irritability with open-label methylphenidate treatment in youth with comorbid attention deficit/hyperactivity disorder and disruptive mood dysregulation disorder. Journal of Child and Adolescent Psychopharmacology 28: 298–305.
+Google Scholar | Crossref | Medline
+World Health Organization (2018) International classification of diseases for mortality and morbidity statistics (11th Revision). Available at: https://icd.who.int/browse11/l-m/en
+Google Scholar
+Wozniak, J, Biederman, J, Kiely, K, et al. (1995) Mania-like symptoms suggestive of childhood-onset bipolar disorder in clinically referred children. Journal of the American Academy of Child and Adolescent Psychiatry 34: 867–876.
+Google Scholar | Crossref | Medline | ISI
+Xu, Y, Farver, JAM, Zhang, Z (2009) Temperament, harsh and indulgent parenting, and Chinese children’s proactive and reactive aggression. Child Development 80: 244–258.
+Google Scholar | Crossref | Medline | ISI</t>
+  </si>
+  <si>
+    <t>ARI references in paper</t>
+  </si>
+  <si>
+    <t>Trauma Reactions in Children with ADHD During the COVID-19 Pandemic: The Mediating Effect of Irritability</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/15325024.2021.1926782</t>
+  </si>
+  <si>
+    <t>Halit Necmi Uçar, Fatih Hilmi Çetin, Serhat Türkoğlu, Gökçeçiçek Arıcı Sağliyan, Özlem Çiçek Zekey &amp; Çiğdem Yılmaz</t>
+  </si>
+  <si>
+    <t>Journal of Loss and Trauma</t>
+  </si>
+  <si>
+    <t>This study aimed to investigate the symptoms of trauma, depression, anxiety, and irritability in children with attention deficit hyperactivity disorder (ADHD) during home confinement due to COVID-19. The sample of this single-center, cross-sectional study consisted of 42 children with ADHD and their parents. There were significant differences in the severity of depression, anxiety, irritability, and ADHD symptoms between the group that experienced pathological trauma reactions and the group that did not. According to the results of mediation analyses, the irritability score was found to be the full mediating factor in the relationship between trauma reaction scores/emotional symptom scores and the severity of ADHD symptoms. Because of the modest sample size due to the exclusion of ADHD patients with comorbidities, we recommend that future research focus on reproducing the role of irritability, in larger samples, as the full mediator on the path from cognition to behavior in children with ADHD under home confinement during the pandemic.</t>
+  </si>
+  <si>
+    <t>Bullying Perpetration and Victimization in Youth: Associations with Irritability and Anxiety</t>
+  </si>
+  <si>
+    <t>Child Psychiatry &amp; Human Development</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10578-021-01192-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior work on has demonstrated that irritability and anxiety are associated with bullying perpetration and victimization, respectively. Even though symptoms of irritability and anxiety often occur concurrently, few studies have tested their interactive effects on perpetration or victimization. The current study recruited 131 youths from a broader program of research that examines the pathophysiology and treatment of pediatric irritability and anxiety. Two moderation tests were performed to examine concurrent irritability and anxiety symptoms and their relation to perpetration and victimization of bullying. More severe anxiety was associated with greater victimization. However, more severe irritability was associated with, not just greater perpetration, but also greater victimization. An irritability-by-anxiety interaction demonstrated that youths with more severe irritability and lower levels of anxiety engaged in more perpetration. Our findings suggest a more nuanced approach to understanding how the commonly comorbid symptoms of irritability and anxiety interact in relation to peer-directed behavior in youths.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hung-Wei Bernie Chen, Erin S. Gardner, Tessa Clarkson, Nicholas R. Eaton, Jillian Lee Wiggins, Ellen Leibenluft &amp; Johanna M. Jarcho </t>
+  </si>
+  <si>
+    <t>Early Predictors of Adolescent Irritability</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.chc.2021.04.002</t>
+  </si>
+  <si>
+    <t>Ellen M. Kessel, Lea R. Dougherty, Samantha Hubacheck, Emma Chad-Friedman, Tom Olino, Gabrielle A. Carlson, Daniel N. Klein,</t>
+  </si>
+  <si>
+    <t>•
+Limited research has examined early precursors/risk factors for adolescent irritability.
+•
+Using multiple methods and informants and a prospective longitudinal design, the authors examined the continuity of irritability from early childhood to adolescence and identified other early predictors of adolescent irritability.
+•
+Across both self-reports and mother-reports, the authors found evidence for continuity of irritability from ages 3 to 15.
+•
+The authors also found that early antecedents of adolescent irritability differ in many instances as a function of either informant or gender.
+•
+The results also suggest that adolescent irritability is characterized by several distinct developmental pathways from age 3 that have the potential to result in an irritable phenotype at age 15.
+•
+They also suggest that self-reported and mother-reported irritability may be capturing distinct underlying constructs, and both should be considered in assessments of adolescent irritability.</t>
+  </si>
+  <si>
+    <t>A Review of the Evidence Base for Psychosocial Interventions for the Treatment of Emotion Dysregulation in Children and Adolescents</t>
+  </si>
+  <si>
+    <t>James G. Waxmonsky, Raman Baweja, Pevitr S. Bansal, Daniel A. Waschbusch</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.chc.2021.04.008</t>
+  </si>
+  <si>
+    <t>KEYWORDS
+_x0001_ Emotion dysregulation _x0001_ Psychosocial treatment _x0001_ Emotion regulation
+_x0001_ Emotion recognition _x0001_ Emotion reactivity _x0001_ Psychotherapy
+KEY POINTS
+_x0001_ Emotion dysregulation (ED) is a transdiagnostic factor that meaningfully increases impairment for a wide range of youth with behavioral health disorders.
+_x0001_ Both modified and unmodified versions of currently available evidence-based psychosocial interventions are associated with reduced levels of ED.
+_x0001_ Little is known about how to personalize the psychosocial treatment of youth with ED
+beyond treating readily identifiable psychiatric comorbidities.
+_x0001_ Future work needs to identify mediational pathways, implement adaptive designs, create
+stepped care pathways integrating psychosocial and pharmacologic treatment, and test
+interventions using multimethod assessment batteries in naturalistic settings.</t>
+  </si>
+  <si>
+    <t>A Modular, Transdiagnostic Approach to Treating Severe Irritability in Children and Adolescents</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.chc.2021.04.011</t>
+  </si>
+  <si>
+    <t>Spencer C. Evans, Lauren Santucci</t>
+  </si>
+  <si>
+    <t>KEYWORDS
+_x0001_ Irritability _x0001_ Mood dysregulation _x0001_ Oppositional _x0001_ Behavioral parent training (BPT)
+_x0001_ Cognitive-behavioral therapy (CBT) _x0001_ Modular _x0001_ Transdiagnostic
+_x0001_ Children and adolescents
+KEY POINTS
+_x0001_ Severe irritability often occurs in youth externalizing and internalizing problems, for which
+behavioral parent training and cognitive-behavioral therapy are recommended
+treatments.
+_x0001_ MATCH is a modular intervention for delivering evidence-based behavioral parent
+training/cognitive-behavioral treatment strategies to youth with anxiety, depression,
+trauma, and/or conduct problems.
+_x0001_ MATCH may be effective in the treatment of severely irritable youth, with strengths
+including its flexible, transdiagnostic, and personalized format.
+_x0001_ We offer strategies for personalized treatment of youth irritability with MATCH, emphasizing behavioral parent training as the first-line approach and cognitive-behavioral treatment elements as complementary or alternative approaches.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.jad.2021.05.037</t>
+  </si>
+  <si>
+    <t>Gianluca Sesso, Annarita Milone, Flavia Drago, Valentina Viglione, Stefano Berloff, Silvia Boldrini, Nina Loriaux, Elena Valente, Agnese Molesti, Francesca Placini, Anna Rita Montesanto, Simone Pisano, Gabriele Masi</t>
+  </si>
+  <si>
+    <t>A novel multidimensional questionnaire for the assessment of emotional dysregulation in adolescents: Reactivity, Intensity, Polarity and Stability questionnaire – youth version (RIPoSt–Y).</t>
+  </si>
+  <si>
+    <t>Background
+The failure to regulate emotions, namely emotional dysregulation (ED), is a relevant construct in adolescent psychiatry, in terms of prognostic and developmental implications. We developed and validated a novel self-report questionnaire for the assessment of ED, the RIPoSt-Y, both in clinical and non-clinical samples.
+Methods
+Items selection and subscales construction were conducted on healthy controls (n=374), while test-retest reliability was evaluated in a subsample (n=72); internal consistency was examined both in the control group and in two clinical samples, respectively including patients with Bipolar Spectrum Disorders (BSD; n=44) and ADHD (n=34). Construct, concurrent and convergent validity were also assessed.
+Results
+Thirty-one items were finally retained, and three subscales were identified (Affective Instability, Emotional Reactivity, Interpersonal Sensitivity). Test-retest was significant for each subscale with moderate-to-good correlations, and internal consistency showed good-to-excellent coefficients. Construct validity was supported by significant differences between patients and controls and gender-related differences. Concurrent validity was confirmed through significant associations with two subscales of the CHT-Q, while convergent validity proved to be significant with the CBCL/YSR dysregulation-profile. Cut-offs were also computed to discriminate clinically significant scores of ED.
+Limitations
+The use of a school-based survey to recruit controls could have biased our results; gender distributions between clinical and non-clinical samples were significantly different.
+Conclusions
+Our novel questionnaire proved to be a valid and reliable tool able to assess the presence of ED in youths and to characterize this fundamental construct in its multidimensional facets.</t>
   </si>
 </sst>
 </file>
@@ -4031,11 +4545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I203"/>
+  <dimension ref="A1:I217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D204" sqref="D204"/>
+      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C218" sqref="C218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9343,6 +9857,370 @@
       </c>
       <c r="H203" s="2" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A204" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="D204" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E204" s="15" t="s">
+        <v>939</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="G204" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H204" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I204" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A205" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="D205" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E205" s="15" t="s">
+        <v>941</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="G205" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H205" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A206" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D206" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E206" s="15" t="s">
+        <v>946</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="G206" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H206" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A207" s="4" t="s">
+        <v>949</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="D207" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E207" s="15" t="s">
+        <v>950</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="G207" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H207" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A208" s="4" t="s">
+        <v>954</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="D208" s="2">
+        <v>2021</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="G208" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H208" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A209" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="D209" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E209" s="15" t="s">
+        <v>960</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="G209" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H209" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A210" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="D210" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E210" s="15" t="s">
+        <v>965</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="G210" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H210" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A211" s="4" t="s">
+        <v>967</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D211" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E211" s="15" t="s">
+        <v>968</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="G211" s="2" t="s">
+        <v>971</v>
+      </c>
+      <c r="H211" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A212" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="D212" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E212" s="15" t="s">
+        <v>973</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="G212" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H212" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A213" s="4" t="s">
+        <v>977</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="D213" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E213" s="15" t="s">
+        <v>979</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="G213" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H213" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A214" s="4" t="s">
+        <v>982</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="D214" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E214" s="15" t="s">
+        <v>983</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="G214" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H214" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I214" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A215" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="D215" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E215" s="15" t="s">
+        <v>988</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="G215" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H215" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A216" s="4" t="s">
+        <v>990</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="D216" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E216" s="15" t="s">
+        <v>991</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="G216" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H216" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A217" s="4" t="s">
+        <v>996</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D217" s="2">
+        <v>2021</v>
+      </c>
+      <c r="E217" s="15" t="s">
+        <v>994</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="G217" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H217" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -9741,8 +10619,35 @@
     <hyperlink ref="E202" r:id="rId389" xr:uid="{9D217C43-8A50-4255-B857-A66D18ED6489}"/>
     <hyperlink ref="E203" r:id="rId390" xr:uid="{7A43D4E4-E73D-4E4F-A730-CDEDB891179B}"/>
     <hyperlink ref="A203" r:id="rId391" xr:uid="{CAEF9400-8900-4325-A280-828F100D8EC7}"/>
+    <hyperlink ref="A204" r:id="rId392" xr:uid="{8E675C53-6B39-45AD-A4B6-6879119A2475}"/>
+    <hyperlink ref="E204" r:id="rId393" xr:uid="{DB364FFA-B443-488F-B997-F3F1B0BCC01C}"/>
+    <hyperlink ref="A205" r:id="rId394" display="Understanding, Assessing, and Intervening with Emotion Dysregulation in Autism Spectrum Disorder" xr:uid="{2BE38CE9-C5BB-4000-B864-BB0025C100BB}"/>
+    <hyperlink ref="E205" r:id="rId395" xr:uid="{E55DBF93-5DAF-4E3B-ACCC-FAF424B5979A}"/>
+    <hyperlink ref="A206" r:id="rId396" xr:uid="{947D89FB-EB88-444D-A8DC-66BFC0BF6BE4}"/>
+    <hyperlink ref="E206" r:id="rId397" xr:uid="{AABDCF44-7994-4811-9629-1C848C0FAC59}"/>
+    <hyperlink ref="A207" r:id="rId398" xr:uid="{9530BE4C-3DBB-40EF-80DE-C974FBB5FA72}"/>
+    <hyperlink ref="E207" r:id="rId399" xr:uid="{FF834AF9-0E08-47F4-8718-2C118834B172}"/>
+    <hyperlink ref="A208" r:id="rId400" display="https://www.researchgate.net/profile/Pascal-Schlechter/publication/332946580_The_Youth_and_Childhood_Adversity_Scale_A_step_towards_developing_a_new_measure_of_adversity_and_its_severity/links/6076d57ca03fca55fe2993a4/The-Youth-and-Childhood-Adversity-Scale-A-step-towards-developing-a-new-measure-of-adversity-and-its-severity.pdf" xr:uid="{5468BEC2-A79C-4C4E-B1EF-FBFD5034AAE1}"/>
+    <hyperlink ref="A209" r:id="rId401" xr:uid="{9BC617CB-F8DB-4C9C-99E1-FEF55A275734}"/>
+    <hyperlink ref="E209" r:id="rId402" xr:uid="{7EFFB5C4-FD24-4A2B-849E-E8E20246A481}"/>
+    <hyperlink ref="E210" r:id="rId403" xr:uid="{1EB42A4C-64B3-430C-A27C-D30DAF3A1799}"/>
+    <hyperlink ref="A210" r:id="rId404" xr:uid="{D2614BBD-E07E-4420-8AF8-93167F842DD6}"/>
+    <hyperlink ref="E211" r:id="rId405" xr:uid="{6BA93832-119B-40C2-9FAF-38D04E667707}"/>
+    <hyperlink ref="A211" r:id="rId406" xr:uid="{2CE8C3F3-C357-4FA2-A75D-88B0F52F03FD}"/>
+    <hyperlink ref="A212" r:id="rId407" xr:uid="{B515BEC3-3370-49CB-9D08-83EEF5A2A4D5}"/>
+    <hyperlink ref="E212" r:id="rId408" xr:uid="{000A5158-3D03-4E83-A000-B7685B5DABE0}"/>
+    <hyperlink ref="E213" r:id="rId409" xr:uid="{154B5C88-CFF6-46F1-9521-FED7D127BFF0}"/>
+    <hyperlink ref="A213" r:id="rId410" xr:uid="{C5E303C9-9B59-4F58-8C71-0096B1BAA97F}"/>
+    <hyperlink ref="E214" r:id="rId411" xr:uid="{EB401A7C-89DE-406D-8A58-50297FB7BA0F}"/>
+    <hyperlink ref="A214" r:id="rId412" xr:uid="{AF7620F8-7B58-4DF5-A5CA-78551F35C449}"/>
+    <hyperlink ref="A215" r:id="rId413" xr:uid="{215B3F94-7B40-4FFF-AAE8-A1B0F0D7C6A9}"/>
+    <hyperlink ref="E215" r:id="rId414" xr:uid="{B3884C1D-8209-47FB-9E8C-1195E75FEB91}"/>
+    <hyperlink ref="E216" r:id="rId415" xr:uid="{EE60D20F-D213-4820-BDA3-87A85FE8EAB0}"/>
+    <hyperlink ref="A216" r:id="rId416" xr:uid="{176F8F47-70F8-4987-9318-FBA556DC37D3}"/>
+    <hyperlink ref="E217" r:id="rId417" xr:uid="{573FE89B-A800-425C-9844-9664C18223E2}"/>
+    <hyperlink ref="A217" r:id="rId418" xr:uid="{8B078612-EE52-4CC2-9C54-AE1D4558504E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId392"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId419"/>
 </worksheet>
 </file>
</xml_diff>